<commit_message>
Re-organize validation info to be more clear
</commit_message>
<xml_diff>
--- a/content/blog/excel_entry/tracking_example_cl.xlsx
+++ b/content/blog/excel_entry/tracking_example_cl.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\crystal_site\content\blog\excel_entry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BCD510C-DFD7-4DB7-A5E5-96D07B91162F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BD9F12-F4C4-4FA9-8DFC-94FD3571014E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{6B88F771-7492-4CBD-B77C-52A0D23D962A}"/>
   </bookViews>
@@ -217,7 +217,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="000"/>
+    <numFmt numFmtId="164" formatCode="000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -262,14 +262,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -833,17 +832,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E9FD89E-FB0A-4EF1-AB5D-0E6CF134659E}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="7" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
@@ -851,14 +850,14 @@
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
     <col min="10" max="10" width="13.140625" customWidth="1"/>
-    <col min="11" max="11" width="27.85546875" style="8" customWidth="1"/>
+    <col min="11" max="11" width="27.85546875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -885,11 +884,11 @@
       <c r="J1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>14088</v>
       </c>
@@ -926,9 +925,8 @@
       <c r="K2" t="s">
         <v>47</v>
       </c>
-      <c r="L2" s="4"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>14091</v>
       </c>
@@ -966,7 +964,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>14099</v>
       </c>
@@ -1002,7 +1000,7 @@
       </c>
       <c r="K4"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>14100</v>
       </c>
@@ -1038,7 +1036,7 @@
       </c>
       <c r="K5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>14200</v>
       </c>
@@ -1074,7 +1072,7 @@
       </c>
       <c r="K6"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>14209</v>
       </c>
@@ -1115,7 +1113,7 @@
     <sortCondition ref="A1:A7"/>
   </sortState>
   <dataConsolidate/>
-  <dataValidations count="7">
+  <dataValidations count="6">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{865AD7FB-A616-4D17-BA70-A4B58D220B74}">
       <formula1>AND(ISNUMBER(A1),COUNTIF($A:$A, A1) = 1, A1 &gt;=14000, A1&lt;=15000)</formula1>
     </dataValidation>
@@ -1125,9 +1123,6 @@
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{4E7DD5BC-2708-41FA-8107-A86A8C07FF7E}">
       <formula1>0</formula1>
       <formula2>30</formula2>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576" xr:uid="{16E1FCA4-CF18-4736-87F9-0F41EC5AE20E}">
-      <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 B8:B1048576" xr:uid="{3B7F04C9-A7EF-4EF2-B246-865A18A3F040}">
       <formula1>TEXT(B1, "00000")</formula1>

</xml_diff>